<commit_message>
working on data formatting for more clear pipeline
</commit_message>
<xml_diff>
--- a/Input_data/NPs/NP_Database.xlsx
+++ b/Input_data/NPs/NP_Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmp95\PycharmProjects\PC_ML_using NetSurfP\Input_data\NPs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pouls\PycharmProjects\PC_ML_using_NSP\Input_data\NPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF878A12-1D13-44DF-B9C2-AAA2C68A84B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D318BE-741C-45EC-9273-8E887E8A7849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
+    <workbookView xWindow="46695" yWindow="6345" windowWidth="21600" windowHeight="11385" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
   </bookViews>
   <sheets>
     <sheet name="NPUNID" sheetId="2" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>BET</t>
   </si>
   <si>
-    <t>RunID</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>200_MNP_BALF100%</t>
+  </si>
+  <si>
+    <t>NPUNID</t>
   </si>
 </sst>
 </file>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD93B0A-7305-43B0-9C03-61303B4AF43A}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,13 +520,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -559,7 +559,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -603,7 +603,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,7 +614,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -647,7 +647,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -658,7 +658,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -680,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,7 +691,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1134,7 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FB506C-18F9-4EF7-A2FE-9BAF44A578A1}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -1178,7 +1178,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -1384,10 +1384,10 @@
         <v>-21</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7">
         <v>378</v>
@@ -1414,7 +1414,7 @@
         <v>25</v>
       </c>
       <c r="N7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1425,10 +1425,10 @@
         <v>-52</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8">
         <v>800</v>
@@ -1455,7 +1455,7 @@
         <v>25</v>
       </c>
       <c r="N8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1466,10 +1466,10 @@
         <v>-11</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9">
         <v>579</v>
@@ -1496,7 +1496,7 @@
         <v>25</v>
       </c>
       <c r="N9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
         <v>25</v>
       </c>
       <c r="N10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding static data as well as new pipeline to work with
</commit_message>
<xml_diff>
--- a/Input_data/NPs/NP_Database.xlsx
+++ b/Input_data/NPs/NP_Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pouls\PycharmProjects\PC_ML_using_NSP\Input_data\NPs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmp95\PycharmProjects\PC_ML_using NetSurfP\Input_data\NPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D318BE-741C-45EC-9273-8E887E8A7849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231B928F-8C42-46DF-AEEC-7A279088447C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46695" yWindow="6345" windowWidth="21600" windowHeight="11385" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
   </bookViews>
   <sheets>
     <sheet name="NPUNID" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>NPID</t>
   </si>
@@ -75,12 +75,6 @@
   </si>
   <si>
     <t>Carboxylate BSA</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>Polystyrene</t>
@@ -509,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD93B0A-7305-43B0-9C03-61303B4AF43A}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -520,13 +514,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -559,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -570,7 +564,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -581,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -592,7 +586,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -603,7 +597,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -625,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -647,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -658,7 +652,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,7 +663,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -680,7 +674,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,7 +685,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,7 +696,7 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1134,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FB506C-18F9-4EF7-A2FE-9BAF44A578A1}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,7 +1157,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1178,7 +1172,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -1190,7 +1184,7 @@
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1212,11 +1206,11 @@
       <c r="G2">
         <v>230</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
       <c r="J2">
         <v>3.2</v>
@@ -1231,7 +1225,7 @@
         <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1242,19 +1236,22 @@
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3">
         <v>353.9</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -1266,7 +1263,7 @@
         <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1278,19 +1275,22 @@
         <v>-24.333333333333332</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4">
         <v>1421</v>
       </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
       </c>
       <c r="K4">
         <v>4</v>
@@ -1302,7 +1302,7 @@
         <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1314,19 +1314,22 @@
         <v>-24.333333333333332</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5">
         <v>2562</v>
       </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
       </c>
       <c r="K5">
         <v>4</v>
@@ -1338,7 +1341,7 @@
         <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1349,19 +1352,22 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <v>2083</v>
       </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
       </c>
       <c r="K6">
         <v>4</v>
@@ -1373,7 +1379,7 @@
         <v>25</v>
       </c>
       <c r="N6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1384,10 +1390,10 @@
         <v>-21</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7">
         <v>378</v>
@@ -1395,11 +1401,11 @@
       <c r="G7">
         <v>410</v>
       </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
       </c>
       <c r="J7">
         <v>62.5</v>
@@ -1414,7 +1420,7 @@
         <v>25</v>
       </c>
       <c r="N7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1425,10 +1431,10 @@
         <v>-52</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F8">
         <v>800</v>
@@ -1436,11 +1442,11 @@
       <c r="G8">
         <v>680</v>
       </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
       </c>
       <c r="J8">
         <v>125</v>
@@ -1455,7 +1461,7 @@
         <v>25</v>
       </c>
       <c r="N8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1466,10 +1472,10 @@
         <v>-11</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9">
         <v>579</v>
@@ -1477,11 +1483,11 @@
       <c r="G9">
         <v>441</v>
       </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
       </c>
       <c r="J9">
         <v>200</v>
@@ -1496,7 +1502,7 @@
         <v>25</v>
       </c>
       <c r="N9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1518,11 +1524,11 @@
       <c r="G10">
         <v>230</v>
       </c>
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" t="s">
-        <v>14</v>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
       </c>
       <c r="J10">
         <v>25</v>
@@ -1537,7 +1543,7 @@
         <v>25</v>
       </c>
       <c r="N10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reformatting and updates to external dataset
</commit_message>
<xml_diff>
--- a/Input_data/NPs/NP_Database.xlsx
+++ b/Input_data/NPs/NP_Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pouls\PycharmProjects\PC_ML_using_NSP\Input_data\NPs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmp95\PycharmProjects\PC_ML_using NetSurfP\Input_data\NPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAA91D4-1298-4257-8020-91A5A5344174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FCAF34-6DB3-4748-A748-44BD96B246CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
   </bookViews>
   <sheets>
     <sheet name="NPUNID" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="84">
   <si>
     <t>NPID</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Dtem</t>
   </si>
   <si>
-    <t>Dh</t>
-  </si>
-  <si>
     <t>Shaken</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Amine</t>
   </si>
   <si>
-    <t>BET</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -150,13 +144,157 @@
   </si>
   <si>
     <t>NPUNID</t>
+  </si>
+  <si>
+    <t>200_PS Carb_10</t>
+  </si>
+  <si>
+    <t>200_PS Carb_100</t>
+  </si>
+  <si>
+    <t>small_Citrate_10</t>
+  </si>
+  <si>
+    <t>large_Citrate_10</t>
+  </si>
+  <si>
+    <t>small_PEI_10</t>
+  </si>
+  <si>
+    <t>large_PEI_10</t>
+  </si>
+  <si>
+    <t>large_PVP@AU_100</t>
+  </si>
+  <si>
+    <t>small_PVP@AU_10</t>
+  </si>
+  <si>
+    <t>small_PVP@AU_100</t>
+  </si>
+  <si>
+    <t>large_Citrate_100</t>
+  </si>
+  <si>
+    <t>large_PEI_100</t>
+  </si>
+  <si>
+    <t>small_Citrate_100</t>
+  </si>
+  <si>
+    <t>small_PEI_100</t>
+  </si>
+  <si>
+    <t>large_PVP@AU_10</t>
+  </si>
+  <si>
+    <t>large_PEG@Au_100</t>
+  </si>
+  <si>
+    <t>large_PEI@Au_100</t>
+  </si>
+  <si>
+    <t>small_PEI@Au_100</t>
+  </si>
+  <si>
+    <t>200_PS Carb@ PEG_100</t>
+  </si>
+  <si>
+    <t>FBS</t>
+  </si>
+  <si>
+    <t>Protein Source</t>
+  </si>
+  <si>
+    <t>BALF</t>
+  </si>
+  <si>
+    <t>Carboxylate</t>
+  </si>
+  <si>
+    <t>PEG 5k</t>
+  </si>
+  <si>
+    <t>Polyethelyenimine</t>
+  </si>
+  <si>
+    <t>Citrate</t>
+  </si>
+  <si>
+    <t>polyvinylpyrrolidone</t>
+  </si>
+  <si>
+    <t>Dh_core</t>
+  </si>
+  <si>
+    <t>Dh_functionalized</t>
+  </si>
+  <si>
+    <t>Raw_FileID</t>
+  </si>
+  <si>
+    <t>200_PS Carb@ PEG_100(b)</t>
+  </si>
+  <si>
+    <t>c200_LS_3C1</t>
+  </si>
+  <si>
+    <t>cMNP_200_30_100</t>
+  </si>
+  <si>
+    <t>cMNP_200_30_5</t>
+  </si>
+  <si>
+    <t>cMNP_200_24_100</t>
+  </si>
+  <si>
+    <t>cMNP_200_5_100</t>
+  </si>
+  <si>
+    <t>c200_LS_3C2</t>
+  </si>
+  <si>
+    <t>c200_LS_3C3</t>
+  </si>
+  <si>
+    <t>50HL</t>
+  </si>
+  <si>
+    <t>50LL</t>
+  </si>
+  <si>
+    <t>50HS</t>
+  </si>
+  <si>
+    <t>50LS</t>
+  </si>
+  <si>
+    <t>200HL</t>
+  </si>
+  <si>
+    <t>200LL</t>
+  </si>
+  <si>
+    <t>200HS</t>
+  </si>
+  <si>
+    <t>200LS</t>
+  </si>
+  <si>
+    <t>cMNP_200_10_24</t>
+  </si>
+  <si>
+    <t>cMNP_200_100_30</t>
+  </si>
+  <si>
+    <t>cMNP_200_5_30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,8 +302,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +320,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -187,18 +335,133 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{FF5A0A4D-9836-48ED-A0F3-E02DD3029105}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -209,6 +472,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E048F05F-71E8-4C64-93E3-98D61C308956}" name="Table1" displayName="Table1" ref="A1:O35" totalsRowShown="0">
+  <autoFilter ref="A1:O35" xr:uid="{E048F05F-71E8-4C64-93E3-98D61C308956}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O29">
+    <sortCondition ref="A1:A29"/>
+  </sortState>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{173B7694-AC4F-448F-AE9B-AF8A1B6CF15E}" name="NPID"/>
+    <tableColumn id="2" xr3:uid="{B4AFAB4A-6882-41B3-8AA5-4A8C9B388892}" name="Zeta Potential"/>
+    <tableColumn id="3" xr3:uid="{0324E036-7D0E-48DC-8A43-D550C12B4897}" name="Core Material" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{3F29D6E2-9845-4948-8891-04A03EAC89B5}" name="Ligand"/>
+    <tableColumn id="6" xr3:uid="{B07F2DCB-7162-4884-AF42-413E4C5C9A70}" name="Dtem"/>
+    <tableColumn id="7" xr3:uid="{6D72242B-4250-44D2-A643-C9E30E7E6259}" name="Dh_core"/>
+    <tableColumn id="8" xr3:uid="{64DEA1B6-3494-4A4C-9E99-737D17B9DADB}" name="Dh_functionalized"/>
+    <tableColumn id="9" xr3:uid="{546409C4-E99C-4804-9742-95397F967656}" name="Shaken"/>
+    <tableColumn id="10" xr3:uid="{3F74D121-1814-44F4-A42C-2BB996DE1C27}" name="Centrifuged"/>
+    <tableColumn id="11" xr3:uid="{1E5D7E63-DC81-492E-BE1D-5F4CFE24426F}" name="Protein Source"/>
+    <tableColumn id="12" xr3:uid="{E3E250E7-C44D-404F-ACBB-563A0C50246A}" name="NP_incubation Concentration (mg/mL)"/>
+    <tableColumn id="13" xr3:uid="{12C54116-DC07-4A62-B593-22B0D11006CC}" name="Incubation Concentration (mg/ml)"/>
+    <tableColumn id="14" xr3:uid="{0D9B1FA5-AEE0-443C-A486-9F058B268244}" name="Incubation Time (minutes)"/>
+    <tableColumn id="15" xr3:uid="{897FC025-BFAE-4349-B965-074E680D9617}" name="Temperature"/>
+    <tableColumn id="16" xr3:uid="{2E2BF4C1-EA9E-40CB-8C6A-16F39B07E599}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,7 +790,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -508,29 +798,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD93B0A-7305-43B0-9C03-61303B4AF43A}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="3" max="4" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -538,10 +831,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D2" s="12">
+        <v>67501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -549,10 +845,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D3" s="13">
+        <v>67502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -560,10 +859,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D4" s="12">
+        <v>67503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -571,10 +873,11 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D5" s="14"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -582,10 +885,11 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="D6" s="14"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -593,10 +897,11 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -604,10 +909,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D8" s="12">
+        <v>72281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -615,10 +923,13 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D9" s="13">
+        <v>72282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -626,10 +937,13 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D10" s="12">
+        <v>72283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -637,10 +951,13 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D11" s="13">
+        <v>72278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -648,10 +965,13 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D12" s="12">
+        <v>72279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -659,10 +979,13 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D13" s="13">
+        <v>72280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -670,10 +993,13 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D14" s="12">
+        <v>72275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -681,10 +1007,13 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D15" s="13">
+        <v>72276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -692,10 +1021,13 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D16" s="12">
+        <v>72277</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -703,240 +1035,537 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D17" s="12">
+        <v>72287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
+        <v>10</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="15">
+        <v>101054</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>11</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="16">
+        <v>101055</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <v>12</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="15">
+        <v>101056</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>13</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="16">
+        <v>101057</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="7">
+        <v>14</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="15">
+        <v>101058</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>15</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="16">
+        <v>101059</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="7">
+        <v>16</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="15">
+        <v>101060</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>17</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="16">
+        <v>101061</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
+        <v>18</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="15">
+        <v>101062</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <v>19</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="16">
+        <v>101063</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
+        <v>20</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="15">
+        <v>101064</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
+        <v>21</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="16">
+        <v>101065</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
+        <v>22</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="15">
+        <v>101066</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>23</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="16">
+        <v>101067</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="7">
+        <v>24</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="15">
+        <v>101068</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5">
+        <v>25</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="16">
+        <v>101069</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" s="7">
+        <v>26</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="15">
+        <v>101070</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" s="5">
+        <v>27</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="16">
+        <v>101071</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" s="9">
+        <v>27</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="15">
+        <v>101072</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="13">
+        <v>67504</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="12">
+        <v>67505</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="13">
+        <v>67506</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" s="7">
+        <v>28</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="12">
+        <v>68393</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" s="5">
+        <v>29</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="12">
+        <v>68395</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" s="7">
+        <v>30</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="13">
+        <v>68396</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" s="5">
+        <v>31</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="12">
+        <v>68397</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C44" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="13">
+        <v>65143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C45" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="12">
+        <v>65141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C46" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" s="13">
+        <v>65142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C47" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="12">
+        <v>65140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" s="7">
+        <v>30</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="13">
+        <v>65139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>32</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="12">
+        <v>65137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" s="7">
+        <v>28</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="13">
+        <v>65138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="12">
+        <v>65136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1133,24 +1762,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FB506C-18F9-4EF7-A2FE-9BAF44A578A1}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="5" width="18" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="38.140625" customWidth="1"/>
-    <col min="11" max="11" width="34.5703125" customWidth="1"/>
-    <col min="12" max="12" width="28.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" customWidth="1"/>
+    <col min="13" max="13" width="28.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1164,37 +1800,40 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1202,15 +1841,15 @@
         <v>-38</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
+      <c r="E2">
+        <v>100</v>
       </c>
       <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
         <v>230</v>
       </c>
       <c r="H2">
@@ -1219,23 +1858,26 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2">
         <v>3.2</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>4</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>30</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>25</v>
       </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1243,40 +1885,44 @@
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E3" s="1">
+        <v>188</v>
       </c>
       <c r="F3" s="1">
-        <v>188</v>
-      </c>
-      <c r="G3" s="1">
         <v>353.9</v>
       </c>
+      <c r="G3" s="1"/>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3">
-        <v>4</v>
+      <c r="J3" t="s">
+        <v>54</v>
       </c>
       <c r="K3">
         <v>4</v>
       </c>
       <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
         <v>30</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>25</v>
       </c>
-      <c r="N3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1285,40 +1931,44 @@
         <v>-24.333333333333332</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E4" s="1">
+        <v>980</v>
       </c>
       <c r="F4" s="1">
-        <v>980</v>
-      </c>
-      <c r="G4" s="1">
         <v>1421</v>
       </c>
+      <c r="G4" s="1"/>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4">
-        <v>4</v>
+      <c r="J4" t="s">
+        <v>54</v>
       </c>
       <c r="K4">
         <v>4</v>
       </c>
       <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
         <v>30</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>25</v>
       </c>
-      <c r="N4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1327,40 +1977,44 @@
         <v>-24.333333333333332</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1810</v>
       </c>
       <c r="F5" s="1">
-        <v>1810</v>
-      </c>
-      <c r="G5" s="1">
         <v>2562</v>
       </c>
+      <c r="G5" s="1"/>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="J5">
-        <v>4</v>
+      <c r="J5" t="s">
+        <v>54</v>
       </c>
       <c r="K5">
         <v>4</v>
       </c>
       <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
         <v>30</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>25</v>
       </c>
-      <c r="N5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1368,40 +2022,44 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E6" s="1">
+        <v>40.5</v>
       </c>
       <c r="F6" s="1">
-        <v>40.5</v>
-      </c>
-      <c r="G6" s="1">
         <v>2083</v>
       </c>
+      <c r="G6" s="1"/>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6">
-        <v>4</v>
+      <c r="J6" t="s">
+        <v>54</v>
       </c>
       <c r="K6">
         <v>4</v>
       </c>
       <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
         <v>30</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>25</v>
       </c>
-      <c r="N6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1409,15 +2067,15 @@
         <v>-21</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>378</v>
       </c>
       <c r="F7">
-        <v>378</v>
-      </c>
-      <c r="G7">
         <v>410</v>
       </c>
       <c r="H7">
@@ -1426,23 +2084,26 @@
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="J7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7">
         <v>62.5</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.2</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>60</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>25</v>
       </c>
-      <c r="N7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1450,40 +2111,43 @@
         <v>-52</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>800</v>
+      </c>
+      <c r="F8">
+        <v>680</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8">
+        <v>125</v>
+      </c>
+      <c r="L8">
+        <v>0.2</v>
+      </c>
+      <c r="M8">
+        <v>60</v>
+      </c>
+      <c r="N8">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s">
         <v>27</v>
       </c>
-      <c r="F8">
-        <v>800</v>
-      </c>
-      <c r="G8">
-        <v>680</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>125</v>
-      </c>
-      <c r="K8">
-        <v>0.2</v>
-      </c>
-      <c r="L8">
-        <v>60</v>
-      </c>
-      <c r="M8">
-        <v>25</v>
-      </c>
-      <c r="N8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1491,15 +2155,15 @@
         <v>-11</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>579</v>
       </c>
       <c r="F9">
-        <v>579</v>
-      </c>
-      <c r="G9">
         <v>441</v>
       </c>
       <c r="H9">
@@ -1508,23 +2172,26 @@
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9">
         <v>200</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.2</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>60</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>25</v>
       </c>
-      <c r="N9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1532,15 +2199,15 @@
         <v>-38</v>
       </c>
       <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
+      <c r="E10">
+        <v>100</v>
       </c>
       <c r="F10">
-        <v>100</v>
-      </c>
-      <c r="G10">
         <v>230</v>
       </c>
       <c r="H10">
@@ -1549,58 +2216,895 @@
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="J10">
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10">
         <v>25</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0.2</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>60</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>25</v>
       </c>
-      <c r="N10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>-63</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11">
+        <v>221</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>30</v>
+      </c>
+      <c r="O11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>-63</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12">
+        <v>221</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12">
+        <v>40</v>
+      </c>
+      <c r="M12">
+        <v>30</v>
+      </c>
+      <c r="O12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>-42</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="4">
+        <v>151</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>30</v>
+      </c>
+      <c r="O13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>-49</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="3">
+        <v>218</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>54</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>30</v>
+      </c>
+      <c r="O14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="2">
+        <v>151</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>30</v>
+      </c>
+      <c r="O15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16">
+        <v>218</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <v>30</v>
+      </c>
+      <c r="O16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17">
+        <v>-11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="2">
+        <v>218</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
+      </c>
+      <c r="L17">
+        <v>40</v>
+      </c>
+      <c r="M17">
+        <v>30</v>
+      </c>
+      <c r="O17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>-12</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="3">
+        <v>151</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <v>30</v>
+      </c>
+      <c r="O18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>-12</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="3">
+        <v>151</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>54</v>
+      </c>
+      <c r="L19">
+        <v>40</v>
+      </c>
+      <c r="M19">
+        <v>30</v>
+      </c>
+      <c r="O19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>-49</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="3">
+        <v>218</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>54</v>
+      </c>
+      <c r="L20">
+        <v>40</v>
+      </c>
+      <c r="M20">
+        <v>30</v>
+      </c>
+      <c r="O20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>39</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="2">
+        <v>218</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>54</v>
+      </c>
+      <c r="L21">
+        <v>40</v>
+      </c>
+      <c r="M21">
+        <v>30</v>
+      </c>
+      <c r="O21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>-42</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="3">
+        <v>151</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22">
+        <v>40</v>
+      </c>
+      <c r="M22">
+        <v>30</v>
+      </c>
+      <c r="O22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>29</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="3">
+        <v>151</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L23">
+        <v>40</v>
+      </c>
+      <c r="M23">
+        <v>30</v>
+      </c>
+      <c r="O23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>-11</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="3">
+        <v>218</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>54</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24">
+        <v>30</v>
+      </c>
+      <c r="O24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>-3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="2">
+        <v>218</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>54</v>
+      </c>
+      <c r="L25">
+        <v>40</v>
+      </c>
+      <c r="M25">
+        <v>30</v>
+      </c>
+      <c r="O25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>12</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="3">
+        <v>218</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>54</v>
+      </c>
+      <c r="L26">
+        <v>40</v>
+      </c>
+      <c r="M26">
+        <v>30</v>
+      </c>
+      <c r="O26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="3">
+        <v>151</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>54</v>
+      </c>
+      <c r="L27">
+        <v>40</v>
+      </c>
+      <c r="M27">
+        <v>30</v>
+      </c>
+      <c r="O27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>-7</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28">
+        <v>266</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>54</v>
+      </c>
+      <c r="L28">
+        <v>40</v>
+      </c>
+      <c r="M28">
+        <v>30</v>
+      </c>
+      <c r="O28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>-38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+      <c r="F29">
+        <v>230</v>
+      </c>
+      <c r="G29">
+        <v>230</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29">
+        <v>3.2</v>
+      </c>
+      <c r="L29">
+        <v>40</v>
+      </c>
+      <c r="M29">
+        <v>30</v>
+      </c>
+      <c r="N29">
+        <v>25</v>
+      </c>
+      <c r="O29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>-38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30">
+        <v>100</v>
+      </c>
+      <c r="F30">
+        <v>230</v>
+      </c>
+      <c r="G30">
+        <v>230</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30">
+        <v>3.2</v>
+      </c>
+      <c r="L30">
+        <v>2</v>
+      </c>
+      <c r="O30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>-38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+      <c r="F31">
+        <v>230</v>
+      </c>
+      <c r="G31">
+        <v>230</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31">
+        <v>3.2</v>
+      </c>
+      <c r="L31">
+        <v>40</v>
+      </c>
+      <c r="O31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>-38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+      <c r="F32">
+        <v>230</v>
+      </c>
+      <c r="G32">
+        <v>230</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>54</v>
+      </c>
+      <c r="K32">
+        <v>3.2</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="O32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>-38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <v>100</v>
+      </c>
+      <c r="F33">
+        <v>230</v>
+      </c>
+      <c r="G33">
+        <v>230</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33">
+        <v>3.2</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="O33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="C35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to try to improve dataset, -need to implement imputation method or switch to human proteome
</commit_message>
<xml_diff>
--- a/Input_data/NPs/NP_Database.xlsx
+++ b/Input_data/NPs/NP_Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmp95\PycharmProjects\PC_ML_using NetSurfP\Input_data\NPs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pouls\PycharmProjects\PC_ML_using_NSP\Input_data\NPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF101D2-BF2B-4FCF-B123-F2274E0BCB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD3C420-61DF-4F95-B1AE-1911ECEC2134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="5445" windowWidth="23325" windowHeight="11055" activeTab="1" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
+    <workbookView xWindow="32445" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
   </bookViews>
   <sheets>
     <sheet name="NPUNID" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="95">
   <si>
     <t>NPID</t>
   </si>
@@ -297,6 +297,30 @@
   </si>
   <si>
     <t>PEG 2k</t>
+  </si>
+  <si>
+    <t>3_</t>
+  </si>
+  <si>
+    <t>4_</t>
+  </si>
+  <si>
+    <t>5_</t>
+  </si>
+  <si>
+    <t>6_</t>
+  </si>
+  <si>
+    <t>7_</t>
+  </si>
+  <si>
+    <t>8_</t>
+  </si>
+  <si>
+    <t>9_</t>
+  </si>
+  <si>
+    <t>Sample_num</t>
   </si>
 </sst>
 </file>
@@ -806,7 +830,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -814,18 +838,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD93B0A-7305-43B0-9C03-61303B4AF43A}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="5" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -833,761 +858,926 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="12">
+      <c r="E2" s="12">
         <v>67501</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="13">
+      <c r="E3" s="13">
         <v>67502</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="12">
+      <c r="E4" s="12">
         <v>67503</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="14">
+      <c r="E5" s="14">
         <v>71435</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="14">
+      <c r="E6" s="14">
         <v>71438</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="14">
+      <c r="E7" s="14">
         <v>71441</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="12">
+      <c r="E8" s="12">
         <v>72281</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="13">
+      <c r="E9" s="13">
         <v>72282</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="12">
+      <c r="E10" s="12">
         <v>72283</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="13">
+      <c r="E11" s="13">
         <v>72278</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>7</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="12">
+      <c r="E12" s="12">
         <v>72279</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="13">
+      <c r="E13" s="13">
         <v>72280</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>8</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="12">
+      <c r="E14" s="12">
         <v>72275</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="13">
+      <c r="E15" s="13">
         <v>72276</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="12">
+      <c r="E16" s="12">
         <v>72277</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="12">
+      <c r="E17" s="12">
         <v>72287</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="7">
         <v>10</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="3">
+        <v>31</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="15">
+      <c r="E18" s="15">
         <v>101054</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="5">
         <v>11</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="2">
+        <v>32</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="16">
+      <c r="E19" s="16">
         <v>101055</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="7">
         <v>12</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="3">
+        <v>33</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="15">
+      <c r="E20" s="15">
         <v>101056</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="5">
         <v>13</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="2">
+        <v>34</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="16">
+      <c r="E21" s="16">
         <v>101057</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="7">
         <v>14</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="3">
+        <v>35</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="15">
+      <c r="E22" s="15">
         <v>101058</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="5">
         <v>15</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="2">
+        <v>36</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="16">
+      <c r="E23" s="16">
         <v>101059</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="7">
         <v>16</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="3">
+        <v>37</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="15">
+      <c r="E24" s="15">
         <v>101060</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="5">
         <v>17</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="2">
+        <v>38</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="16">
+      <c r="E25" s="16">
         <v>101061</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="7">
         <v>18</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="3">
+        <v>39</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="15">
+      <c r="E26" s="15">
         <v>101062</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="5">
         <v>19</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="2">
+        <v>40</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="16">
+      <c r="E27" s="16">
         <v>101063</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="7">
         <v>20</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="3">
+        <v>41</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="15">
+      <c r="E28" s="15">
         <v>101064</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="5">
         <v>21</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="2">
+        <v>42</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="16">
+      <c r="E29" s="16">
         <v>101065</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="7">
         <v>22</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="3">
+        <v>43</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="15">
+      <c r="E30" s="15">
         <v>101066</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="5">
         <v>23</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="2">
+        <v>44</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="16">
+      <c r="E31" s="16">
         <v>101067</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="7">
         <v>24</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="3">
+        <v>45</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="15">
+      <c r="E32" s="15">
         <v>101068</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="5">
         <v>25</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="2">
+        <v>46</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="16">
+      <c r="E33" s="16">
         <v>101069</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="7">
         <v>26</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="3">
+        <v>47</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="15">
+      <c r="E34" s="15">
         <v>101070</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="5">
         <v>27</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="2">
+        <v>48</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="16">
+      <c r="E35" s="16">
         <v>101071</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="9">
         <v>27</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36">
+        <v>49</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="15">
+      <c r="E36" s="15">
         <v>101072</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37">
+        <v>79</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="13">
+      <c r="E37" s="13">
         <v>67504</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38">
+        <v>80</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="12">
+      <c r="E38" s="12">
         <v>67505</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39">
+        <v>81</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="13">
+      <c r="E39" s="13">
         <v>67506</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="7">
         <v>28</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="3">
+        <v>68</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="12">
+      <c r="E40" s="12">
         <v>68393</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="5">
         <v>29</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="2">
+        <v>70</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="12">
+      <c r="E41" s="12">
         <v>68395</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="7">
         <v>30</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="3">
+        <v>71</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="13">
+      <c r="E42" s="13">
         <v>68396</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="5">
         <v>31</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="2">
+        <v>72</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="12">
+      <c r="E43" s="12">
         <v>68397</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="B44" s="5">
+        <v>33</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="13">
+      <c r="E44" s="13">
         <v>65143</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="B45" s="7">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D45" s="12">
+      <c r="E45" s="12">
         <v>65141</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="B46" s="5">
+        <v>35</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="13">
+      <c r="E46" s="13">
         <v>65142</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="B47" s="7">
+        <v>36</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D47" s="12">
+      <c r="E47" s="12">
         <v>65140</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="7">
         <v>30</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="13">
+      <c r="E48" s="13">
         <v>65139</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
         <v>32</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="12">
+      <c r="E49" s="12">
         <v>65137</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="7">
         <v>28</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D50" s="13">
+      <c r="E50" s="13">
         <v>65138</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="12">
+      <c r="E51" s="12">
         <v>65136</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1786,7 +1976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FB506C-18F9-4EF7-A2FE-9BAF44A578A1}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>

</xml_diff>